<commit_message>
Diese Änderungen wurden bereits im vorherigen Upload beschrieben
</commit_message>
<xml_diff>
--- a/P2_Personalverwaltung/data/Gehaltstabelle.xlsx
+++ b/P2_Personalverwaltung/data/Gehaltstabelle.xlsx
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>